<commit_message>
Executed Login and Sign up script by testng.xml file
</commit_message>
<xml_diff>
--- a/TestData/UserData.xlsx
+++ b/TestData/UserData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB7CF5E-39A6-4685-96BD-2E6389579C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E198550A-8AE5-4DF9-8403-B166E5B68666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="5" r:id="rId1"/>
@@ -116,22 +116,22 @@
     <t>Gujarat</t>
   </si>
   <si>
-    <t>rajnish@asite.com</t>
-  </si>
-  <si>
-    <t>deppak@asite.com</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Raj</t>
-  </si>
-  <si>
-    <t>Geta</t>
-  </si>
-  <si>
-    <t>getta@gmail.com</t>
+    <t>sehat@asite.com</t>
+  </si>
+  <si>
+    <t>narayan@asite.com</t>
+  </si>
+  <si>
+    <t>abhishek@asite.com</t>
+  </si>
+  <si>
+    <t>Sehat</t>
+  </si>
+  <si>
+    <t>abhishek</t>
+  </si>
+  <si>
+    <t>narayn</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -217,6 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,13 +502,13 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -537,10 +538,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -560,10 +561,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -583,10 +584,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
         <v>35</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -595,10 +596,10 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Newly Added Test Data in excel file
</commit_message>
<xml_diff>
--- a/TestData/UserData.xlsx
+++ b/TestData/UserData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53706FBF-1539-4073-A42D-0DBFFA2A18CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F709071-899F-4E83-9F19-C91FD215B1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,25 +113,25 @@
     <t>Gujarat</t>
   </si>
   <si>
-    <t>gopalesh</t>
-  </si>
-  <si>
-    <t>gopal@asite.com</t>
-  </si>
-  <si>
-    <t>samara</t>
-  </si>
-  <si>
-    <t>samara@asite.com</t>
-  </si>
-  <si>
-    <t>virpal</t>
-  </si>
-  <si>
-    <t>virpal@asite.com</t>
-  </si>
-  <si>
     <t>Window Testing</t>
+  </si>
+  <si>
+    <t>Govind Patel</t>
+  </si>
+  <si>
+    <t>govind@asite.com</t>
+  </si>
+  <si>
+    <t>Namrata Shah</t>
+  </si>
+  <si>
+    <t>namrata@asite.com</t>
+  </si>
+  <si>
+    <t>Gajendra Rathod</t>
+  </si>
+  <si>
+    <t>gajendra@asite.com</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -217,6 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,7 +502,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,16 +538,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
         <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>27</v>
@@ -560,10 +561,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
         <v>32</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -583,10 +584,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
         <v>34</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Updated Test Data for signup
</commit_message>
<xml_diff>
--- a/TestData/UserData.xlsx
+++ b/TestData/UserData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F709071-899F-4E83-9F19-C91FD215B1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163A9D7E-A397-4276-8D1C-126855BAA0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Selenium</t>
   </si>
@@ -119,19 +119,22 @@
     <t>Govind Patel</t>
   </si>
   <si>
-    <t>govind@asite.com</t>
-  </si>
-  <si>
     <t>Namrata Shah</t>
   </si>
   <si>
-    <t>namrata@asite.com</t>
-  </si>
-  <si>
     <t>Gajendra Rathod</t>
   </si>
   <si>
     <t>gajendra@asite.com</t>
+  </si>
+  <si>
+    <t>govind1@asite.com</t>
+  </si>
+  <si>
+    <t>namrata2@asite.com</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
   </si>
 </sst>
 </file>
@@ -217,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -502,7 +505,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +544,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -561,10 +564,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -584,16 +587,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -606,6 +609,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{956BCE3B-B5BE-4D86-8C86-224679341041}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{63E80F7D-D550-47DF-B4DF-EAB71DF902CB}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{893DCF54-768D-4BE4-8CC3-BCE9F6A8251A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>